<commit_message>
aspose and excel working
</commit_message>
<xml_diff>
--- a/excel1.xlsx
+++ b/excel1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IdeaProjectsOnE\JavaBlueProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +39,12 @@
   </si>
   <si>
     <t>xx</t>
+  </si>
+  <si>
+    <t>ieri</t>
+  </si>
+  <si>
+    <t>aa</t>
   </si>
 </sst>
 </file>
@@ -107,6 +118,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -154,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -432,6 +446,20 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -446,7 +474,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -458,7 +486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>